<commit_message>
Including mother and kids in the map.
</commit_message>
<xml_diff>
--- a/Character Map.xlsx
+++ b/Character Map.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="309">
   <si>
     <t>Name</t>
   </si>
@@ -523,7 +523,7 @@
     <t>Pandu, Surya</t>
   </si>
   <si>
-    <t>(Yudhishthira, Bhim, Arjun), Karna</t>
+    <t>Yudhishthira, Bhim, Arjun, Karna</t>
   </si>
   <si>
     <t>Kutighata</t>
@@ -565,7 +565,7 @@
     <t>Muni</t>
   </si>
   <si>
-    <t>Bhimasena, Ugrasena, Suparna, Varuna, Gopati, Dhritarashtra, Suryavarcha, Pattravana, Arkapana, Prayuta, Bhima, Chitraratha, Shalishira, Pradyumna, Kali, Narada</t>
+    <t>Bhimasena, Ugrasena, Suparna, Varuna2, Gopati, Dhritarashtra(2), Suryavarcha, Pattravana, Arkapana, Prayuta, Bhima2, Chitraratha, Shalishira, Pradyumna, Kali, Narada</t>
   </si>
   <si>
     <t>Nabhaga</t>
@@ -605,9 +605,6 @@
   </si>
   <si>
     <t>Kunti, Madri</t>
-  </si>
-  <si>
-    <t>(Yudhishthira, Bhim, Arjun), (Nakul, Sahadeva)</t>
   </si>
   <si>
     <t>Parashuram</t>
@@ -757,10 +754,7 @@
     <t>Parikshit put dead snake on his shoulders</t>
   </si>
   <si>
-    <t>_, Ganga</t>
-  </si>
-  <si>
-    <t>(Pandu, Dhritarashtra, Vidura), (Bhishma)</t>
+    <t>Pandu, Dhritarashtra, Vidura, Bhishma</t>
   </si>
   <si>
     <t>Sharabha</t>
@@ -4966,7 +4960,7 @@
         <v>197</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="I98" s="6"/>
       <c r="J98" s="6"/>
@@ -4993,14 +4987,14 @@
     </row>
     <row r="99">
       <c r="A99" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C99" s="6"/>
       <c r="D99" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E99" s="6"/>
       <c r="F99" s="6"/>
@@ -5031,7 +5025,7 @@
     </row>
     <row r="100">
       <c r="A100" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>34</v>
@@ -5080,14 +5074,14 @@
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
       <c r="H101" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I101" s="6"/>
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
       <c r="M101" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N101" s="6"/>
       <c r="O101" s="5" t="s">
@@ -5111,7 +5105,7 @@
     </row>
     <row r="102">
       <c r="A102" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>34</v>
@@ -5149,7 +5143,7 @@
     </row>
     <row r="103">
       <c r="A103" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -5185,7 +5179,7 @@
     </row>
     <row r="104">
       <c r="A104" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>34</v>
@@ -5223,7 +5217,7 @@
     </row>
     <row r="105">
       <c r="A105" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>34</v>
@@ -5261,7 +5255,7 @@
     </row>
     <row r="106">
       <c r="A106" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -5274,10 +5268,10 @@
       <c r="J106" s="6"/>
       <c r="K106" s="6"/>
       <c r="L106" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M106" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N106" s="6"/>
       <c r="O106" s="6"/>
@@ -5299,7 +5293,7 @@
     </row>
     <row r="107">
       <c r="A107" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>34</v>
@@ -5337,7 +5331,7 @@
     </row>
     <row r="108">
       <c r="A108" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>34</v>
@@ -5375,7 +5369,7 @@
     </row>
     <row r="109">
       <c r="A109" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -5386,12 +5380,12 @@
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
       <c r="H109" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
       <c r="K109" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L109" s="6"/>
       <c r="M109" s="6"/>
@@ -5415,7 +5409,7 @@
     </row>
     <row r="110">
       <c r="A110" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>34</v>
@@ -5453,12 +5447,12 @@
     </row>
     <row r="111">
       <c r="A111" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>177</v>
@@ -5468,7 +5462,7 @@
         <v>135</v>
       </c>
       <c r="H111" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I111" s="6"/>
       <c r="J111" s="6"/>
@@ -5539,7 +5533,7 @@
     </row>
     <row r="113">
       <c r="A113" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>34</v>
@@ -5577,7 +5571,7 @@
     </row>
     <row r="114">
       <c r="A114" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>34</v>
@@ -5615,7 +5609,7 @@
     </row>
     <row r="115">
       <c r="A115" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>34</v>
@@ -5653,7 +5647,7 @@
     </row>
     <row r="116">
       <c r="A116" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>34</v>
@@ -5691,7 +5685,7 @@
     </row>
     <row r="117">
       <c r="A117" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -5699,7 +5693,7 @@
       <c r="E117" s="6"/>
       <c r="F117" s="5"/>
       <c r="G117" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H117" s="6"/>
       <c r="I117" s="6"/>
@@ -5727,7 +5721,7 @@
     </row>
     <row r="118">
       <c r="A118" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>34</v>
@@ -5765,7 +5759,7 @@
     </row>
     <row r="119">
       <c r="A119" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -5788,7 +5782,7 @@
       <c r="R119" s="5"/>
       <c r="S119" s="5"/>
       <c r="T119" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U119" s="6"/>
       <c r="V119" s="6"/>
@@ -5841,7 +5835,7 @@
     </row>
     <row r="121">
       <c r="A121" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -5889,10 +5883,10 @@
       </c>
       <c r="F122" s="5"/>
       <c r="G122" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I122" s="6"/>
       <c r="J122" s="6"/>
@@ -5919,7 +5913,7 @@
     </row>
     <row r="123">
       <c r="A123" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>34</v>
@@ -5957,7 +5951,7 @@
     </row>
     <row r="124">
       <c r="A124" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>187</v>
@@ -5999,12 +5993,12 @@
     </row>
     <row r="125">
       <c r="A125" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E125" s="6"/>
       <c r="F125" s="6"/>
@@ -6035,7 +6029,7 @@
     </row>
     <row r="126">
       <c r="A126" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -6071,7 +6065,7 @@
     </row>
     <row r="127">
       <c r="A127" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>34</v>
@@ -6109,13 +6103,13 @@
     </row>
     <row r="128">
       <c r="A128" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
       <c r="D128" s="5"/>
       <c r="E128" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F128" s="6"/>
       <c r="G128" s="5"/>
@@ -6145,7 +6139,7 @@
     </row>
     <row r="129">
       <c r="A129" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -6183,20 +6177,20 @@
     </row>
     <row r="130">
       <c r="A130" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B130" s="6"/>
       <c r="C130" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
       <c r="F130" s="6"/>
       <c r="G130" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="H130" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="H130" s="5" t="s">
-        <v>241</v>
       </c>
       <c r="I130" s="6"/>
       <c r="J130" s="6"/>
@@ -6223,14 +6217,14 @@
     </row>
     <row r="131">
       <c r="A131" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>74</v>
       </c>
       <c r="C131" s="6"/>
       <c r="D131" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E131" s="6"/>
       <c r="F131" s="6"/>
@@ -6261,11 +6255,11 @@
     </row>
     <row r="132">
       <c r="A132" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B132" s="6"/>
       <c r="C132" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>121</v>
@@ -6299,7 +6293,7 @@
     </row>
     <row r="133">
       <c r="A133" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>34</v>
@@ -6337,7 +6331,7 @@
     </row>
     <row r="134">
       <c r="A134" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
@@ -6382,7 +6376,7 @@
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
       <c r="H135" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I135" s="6"/>
       <c r="J135" s="6"/>
@@ -6398,7 +6392,7 @@
       <c r="R135" s="6"/>
       <c r="S135" s="6"/>
       <c r="T135" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="U135" s="6"/>
       <c r="V135" s="6"/>
@@ -6421,10 +6415,10 @@
       <c r="E136" s="6"/>
       <c r="F136" s="6"/>
       <c r="G136" s="5" t="s">
-        <v>248</v>
+        <v>73</v>
       </c>
       <c r="H136" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I136" s="6"/>
       <c r="J136" s="6"/>
@@ -6451,7 +6445,7 @@
     </row>
     <row r="137">
       <c r="A137" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>34</v>
@@ -6489,7 +6483,7 @@
     </row>
     <row r="138">
       <c r="A138" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>34</v>
@@ -6527,7 +6521,7 @@
     </row>
     <row r="139">
       <c r="A139" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
@@ -6563,7 +6557,7 @@
     </row>
     <row r="140">
       <c r="A140" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
@@ -6597,7 +6591,7 @@
     </row>
     <row r="141">
       <c r="A141" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>34</v>
@@ -6635,7 +6629,7 @@
     </row>
     <row r="142">
       <c r="A142" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>34</v>
@@ -6662,7 +6656,7 @@
       <c r="R142" s="6"/>
       <c r="S142" s="6"/>
       <c r="T142" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="U142" s="6"/>
       <c r="V142" s="6"/>
@@ -6677,7 +6671,7 @@
     </row>
     <row r="143">
       <c r="A143" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>34</v>
@@ -6715,11 +6709,11 @@
     </row>
     <row r="144">
       <c r="A144" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B144" s="6"/>
       <c r="C144" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D144" s="6"/>
       <c r="E144" s="6"/>
@@ -6751,7 +6745,7 @@
     </row>
     <row r="145">
       <c r="A145" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>34</v>
@@ -6789,7 +6783,7 @@
     </row>
     <row r="146">
       <c r="A146" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
@@ -6797,7 +6791,7 @@
         <v>124</v>
       </c>
       <c r="E146" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
@@ -6829,7 +6823,7 @@
     </row>
     <row r="147">
       <c r="A147" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
@@ -6837,7 +6831,7 @@
       <c r="E147" s="6"/>
       <c r="F147" s="5"/>
       <c r="G147" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H147" s="6"/>
       <c r="I147" s="6"/>
@@ -6865,7 +6859,7 @@
     </row>
     <row r="148">
       <c r="A148" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -6874,7 +6868,7 @@
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
       <c r="H148" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I148" s="6"/>
       <c r="J148" s="6"/>
@@ -6901,7 +6895,7 @@
     </row>
     <row r="149">
       <c r="A149" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
@@ -6937,7 +6931,7 @@
     </row>
     <row r="150">
       <c r="A150" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
@@ -6948,7 +6942,7 @@
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
       <c r="H150" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I150" s="6"/>
       <c r="J150" s="6"/>
@@ -6975,7 +6969,7 @@
     </row>
     <row r="151">
       <c r="A151" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>34</v>
@@ -7022,11 +7016,11 @@
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
       <c r="H152" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I152" s="6"/>
       <c r="J152" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K152" s="6"/>
       <c r="L152" s="6"/>
@@ -7089,7 +7083,7 @@
     </row>
     <row r="154">
       <c r="A154" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B154" s="5" t="s">
         <v>34</v>
@@ -7127,7 +7121,7 @@
     </row>
     <row r="155">
       <c r="A155" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B155" s="5" t="s">
         <v>34</v>
@@ -7165,7 +7159,7 @@
     </row>
     <row r="156">
       <c r="A156" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B156" s="5" t="s">
         <v>74</v>
@@ -7175,12 +7169,12 @@
         <v>135</v>
       </c>
       <c r="E156" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
       <c r="H156" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I156" s="6"/>
       <c r="J156" s="6"/>
@@ -7207,7 +7201,7 @@
     </row>
     <row r="157">
       <c r="A157" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B157" s="5" t="s">
         <v>34</v>
@@ -7249,7 +7243,7 @@
       </c>
       <c r="B158" s="6"/>
       <c r="C158" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
@@ -7323,7 +7317,7 @@
     </row>
     <row r="160">
       <c r="A160" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
@@ -7357,10 +7351,10 @@
     </row>
     <row r="161">
       <c r="A161" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C161" s="6"/>
       <c r="D161" s="6"/>
@@ -7380,7 +7374,7 @@
       <c r="R161" s="6"/>
       <c r="S161" s="6"/>
       <c r="T161" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="U161" s="6"/>
       <c r="V161" s="6"/>
@@ -7395,7 +7389,7 @@
     </row>
     <row r="162">
       <c r="A162" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B162" s="5" t="s">
         <v>34</v>
@@ -7433,11 +7427,11 @@
     </row>
     <row r="163">
       <c r="A163" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B163" s="6"/>
       <c r="D163" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
@@ -7468,7 +7462,7 @@
     </row>
     <row r="164">
       <c r="A164" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
@@ -7507,19 +7501,19 @@
         <v>31</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C165" s="6"/>
       <c r="D165" s="5" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
       <c r="G165" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H165" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I165" s="6"/>
       <c r="J165" s="6"/>
@@ -7535,7 +7529,7 @@
       <c r="R165" s="6"/>
       <c r="S165" s="6"/>
       <c r="T165" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="U165" s="6"/>
       <c r="V165" s="6"/>
@@ -7550,7 +7544,7 @@
     </row>
     <row r="166">
       <c r="A166" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B166" s="5" t="s">
         <v>134</v>
@@ -7560,7 +7554,7 @@
       <c r="E166" s="6"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H166" s="6"/>
       <c r="I166" s="6"/>
@@ -7626,7 +7620,7 @@
     </row>
     <row r="168">
       <c r="A168" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
@@ -7660,7 +7654,7 @@
     </row>
     <row r="169">
       <c r="A169" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -7699,7 +7693,7 @@
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E170" s="6"/>
       <c r="F170" s="5"/>
@@ -7732,11 +7726,11 @@
     </row>
     <row r="171">
       <c r="A171" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B171" s="6"/>
       <c r="C171" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D171" s="6"/>
       <c r="E171" s="6"/>
@@ -7810,7 +7804,7 @@
     </row>
     <row r="173">
       <c r="A173" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
@@ -7846,7 +7840,7 @@
     </row>
     <row r="174">
       <c r="A174" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -7860,13 +7854,13 @@
         <v>20</v>
       </c>
       <c r="K174" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L174" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M174" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N174" s="6"/>
       <c r="O174" s="6"/>
@@ -7874,7 +7868,7 @@
       <c r="Q174" s="6"/>
       <c r="R174" s="6"/>
       <c r="S174" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T174" s="6"/>
       <c r="U174" s="6"/>
@@ -7890,7 +7884,7 @@
     </row>
     <row r="175">
       <c r="A175" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B175" s="5" t="s">
         <v>34</v>
@@ -7928,7 +7922,7 @@
     </row>
     <row r="176">
       <c r="A176" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B176" s="5" t="s">
         <v>34</v>
@@ -7966,7 +7960,7 @@
     </row>
     <row r="177">
       <c r="A177" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
@@ -8004,7 +7998,7 @@
     </row>
     <row r="178">
       <c r="A178" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B178" s="5" t="s">
         <v>34</v>
@@ -8055,7 +8049,7 @@
         <v>37</v>
       </c>
       <c r="H179" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="I179" s="6"/>
       <c r="J179" s="6"/>
@@ -8089,7 +8083,7 @@
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
       <c r="D180" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="6"/>
@@ -8122,7 +8116,7 @@
     </row>
     <row r="181">
       <c r="A181" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B181" s="5" t="s">
         <v>34</v>
@@ -8164,7 +8158,7 @@
       </c>
       <c r="B182" s="6"/>
       <c r="C182" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
@@ -8196,7 +8190,7 @@
     </row>
     <row r="183">
       <c r="A183" s="5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
@@ -8207,7 +8201,7 @@
         <v>177</v>
       </c>
       <c r="H183" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I183" s="6"/>
       <c r="J183" s="6"/>
@@ -8234,27 +8228,27 @@
     </row>
     <row r="184">
       <c r="A184" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B184" s="6"/>
       <c r="C184" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E184" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F184" s="6"/>
       <c r="G184" s="6"/>
       <c r="H184" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I184" s="6"/>
       <c r="J184" s="6"/>
       <c r="K184" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="L184" s="6"/>
       <c r="M184" s="6"/>
@@ -8280,7 +8274,7 @@
     </row>
     <row r="185">
       <c r="A185" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -8314,7 +8308,7 @@
     </row>
     <row r="186">
       <c r="A186" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
@@ -8348,7 +8342,7 @@
     </row>
     <row r="187">
       <c r="A187" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
@@ -8357,7 +8351,7 @@
       <c r="F187" s="6"/>
       <c r="G187" s="6"/>
       <c r="H187" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="I187" s="6"/>
       <c r="J187" s="6"/>
@@ -8384,12 +8378,12 @@
     </row>
     <row r="188">
       <c r="A188" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>45</v>

</xml_diff>